<commit_message>
-- lập biên bản báo cáo kiểm kê
</commit_message>
<xml_diff>
--- a/storage/app/public/data/danhsachvattu.xlsx
+++ b/storage/app/public/data/danhsachvattu.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\v20\storage\app\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\20V\storage\app\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="169">
   <si>
     <t>Tên vật tư y tế</t>
   </si>
@@ -967,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I247" sqref="I247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3646,6 +3646,3157 @@
       </c>
       <c r="G115" s="17">
         <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A116" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D116" s="4">
+        <v>10</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G116" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A117" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B117" s="4">
+        <v>90407219</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D117" s="4">
+        <v>10</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A118" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B118" s="4">
+        <v>6410419</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D118" s="4">
+        <v>10</v>
+      </c>
+      <c r="E118" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G118" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A119" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B119" s="6">
+        <v>6414810</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D119" s="4">
+        <v>10</v>
+      </c>
+      <c r="E119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F119" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A120" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B120" s="4">
+        <v>42411608</v>
+      </c>
+      <c r="C120" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D120" s="4">
+        <v>10</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F120" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G120" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A121" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="4">
+        <v>10</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G121" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A122" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D122" s="4">
+        <v>10</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G122" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A123" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D123" s="4">
+        <v>10</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G123" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A124" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D124" s="4">
+        <v>10</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G124" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A125" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D125" s="4">
+        <v>10</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G125" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A126" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" s="4">
+        <v>10</v>
+      </c>
+      <c r="E126" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G126" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A127" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" s="4">
+        <v>10</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G127" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A128" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D128" s="4">
+        <v>10</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F128" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G128" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A129" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129" s="4">
+        <v>10</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G129" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A130" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D130" s="4">
+        <v>10</v>
+      </c>
+      <c r="E130" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F130" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G130" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A131" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131" s="4">
+        <v>10</v>
+      </c>
+      <c r="E131" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G131" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A132" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" s="4">
+        <v>10</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F132" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G132" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A133" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133" s="4">
+        <v>10</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F133" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G133" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A134" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D134" s="4">
+        <v>10</v>
+      </c>
+      <c r="E134" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G134" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A135" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D135" s="4">
+        <v>10</v>
+      </c>
+      <c r="E135" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F135" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G135" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A136" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136" s="4">
+        <v>10</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F136" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G136" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A137" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C137" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" s="4">
+        <v>10</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G137" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A138" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C138" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D138" s="4">
+        <v>10</v>
+      </c>
+      <c r="E138" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G138" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A139" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D139" s="4">
+        <v>10</v>
+      </c>
+      <c r="E139" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G139" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A140" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D140" s="4">
+        <v>10</v>
+      </c>
+      <c r="E140" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G140" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A141" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B141" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D141" s="4">
+        <v>10</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G141" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A142" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D142" s="4">
+        <v>10</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G142" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A143" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C143" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D143" s="4">
+        <v>10</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G143" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A144" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B144" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C144" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" s="4">
+        <v>10</v>
+      </c>
+      <c r="E144" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F144" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G144" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A145" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B145" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C145" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145" s="4">
+        <v>10</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F145" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G145" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A146" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B146" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C146" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" s="4">
+        <v>10</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G146" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A147" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B147" s="6">
+        <v>6005500030</v>
+      </c>
+      <c r="C147" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D147" s="4">
+        <v>10</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F147" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G147" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A148" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B148" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" s="4">
+        <v>10</v>
+      </c>
+      <c r="E148" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G148" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A149" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D149" s="4">
+        <v>10</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F149" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G149" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A150" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C150" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D150" s="4">
+        <v>10</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G150" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A151" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B151" s="6">
+        <v>326</v>
+      </c>
+      <c r="C151" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D151" s="4">
+        <v>10</v>
+      </c>
+      <c r="E151" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G151" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A152" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B152" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D152" s="4">
+        <v>10</v>
+      </c>
+      <c r="E152" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F152" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G152" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A153" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B153" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D153" s="4">
+        <v>10</v>
+      </c>
+      <c r="E153" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F153" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G153" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A154" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B154" s="6">
+        <v>4163214</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D154" s="4">
+        <v>10</v>
+      </c>
+      <c r="E154" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F154" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G154" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A155" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B155" s="6">
+        <v>503853</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D155" s="4">
+        <v>10</v>
+      </c>
+      <c r="E155" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F155" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G155" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A156" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B156" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D156" s="4">
+        <v>10</v>
+      </c>
+      <c r="E156" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G156" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A157" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B157" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D157" s="4">
+        <v>10</v>
+      </c>
+      <c r="E157" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F157" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G157" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A158" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B158" s="6">
+        <v>503852</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D158" s="4">
+        <v>10</v>
+      </c>
+      <c r="E158" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G158" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A159" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B159" s="6">
+        <v>550197</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D159" s="4">
+        <v>10</v>
+      </c>
+      <c r="E159" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F159" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G159" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+      <c r="A160" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B160" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D160" s="4">
+        <v>10</v>
+      </c>
+      <c r="E160" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G160" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A161" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B161" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C161" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D161" s="4">
+        <v>10</v>
+      </c>
+      <c r="E161" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F161" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G161" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A162" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B162" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D162" s="4">
+        <v>10</v>
+      </c>
+      <c r="E162" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G162" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A163" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B163" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C163" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D163" s="4">
+        <v>10</v>
+      </c>
+      <c r="E163" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F163" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G163" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A164" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B164" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C164" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D164" s="4">
+        <v>10</v>
+      </c>
+      <c r="E164" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F164" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G164" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A165" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B165" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C165" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D165" s="4">
+        <v>10</v>
+      </c>
+      <c r="E165" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F165" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G165" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A166" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B166" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D166" s="4">
+        <v>10</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F166" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G166" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A167" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B167" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C167" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D167" s="4">
+        <v>10</v>
+      </c>
+      <c r="E167" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G167" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A168" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B168" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D168" s="4">
+        <v>10</v>
+      </c>
+      <c r="E168" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G168" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A169" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D169" s="4">
+        <v>10</v>
+      </c>
+      <c r="E169" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G169" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A170" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B170" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D170" s="4">
+        <v>10</v>
+      </c>
+      <c r="E170" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G170" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A171" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B171" s="6">
+        <v>5030850</v>
+      </c>
+      <c r="C171" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D171" s="4">
+        <v>10</v>
+      </c>
+      <c r="E171" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G171" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A172" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B172" s="6">
+        <v>5030850</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D172" s="4">
+        <v>10</v>
+      </c>
+      <c r="E172" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F172" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G172" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A173" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D173" s="4">
+        <v>10</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F173" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G173" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A174" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D174" s="4">
+        <v>10</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F174" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G174" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A175" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D175" s="4">
+        <v>10</v>
+      </c>
+      <c r="E175" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G175" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A176" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B176" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D176" s="4">
+        <v>10</v>
+      </c>
+      <c r="E176" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F176" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G176" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A177" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D177" s="4">
+        <v>10</v>
+      </c>
+      <c r="E177" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G177" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A178" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D178" s="4">
+        <v>10</v>
+      </c>
+      <c r="E178" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G178" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A179" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B179" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D179" s="4">
+        <v>10</v>
+      </c>
+      <c r="E179" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G179" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A180" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D180" s="4">
+        <v>10</v>
+      </c>
+      <c r="E180" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G180" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A181" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C181" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D181" s="4">
+        <v>10</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G181" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A182" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B182" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C182" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D182" s="4">
+        <v>10</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F182" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G182" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A183" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B183" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C183" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D183" s="4">
+        <v>10</v>
+      </c>
+      <c r="E183" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F183" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G183" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A184" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B184" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C184" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D184" s="4">
+        <v>10</v>
+      </c>
+      <c r="E184" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F184" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G184" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A185" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D185" s="4">
+        <v>10</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F185" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G185" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A186" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B186" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C186" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D186" s="4">
+        <v>10</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F186" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G186" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A187" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B187" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D187" s="4">
+        <v>10</v>
+      </c>
+      <c r="E187" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F187" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G187" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A188" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B188" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D188" s="4">
+        <v>10</v>
+      </c>
+      <c r="E188" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F188" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G188" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A189" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C189" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D189" s="4">
+        <v>10</v>
+      </c>
+      <c r="E189" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F189" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G189" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A190" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B190" s="6">
+        <v>6005500030</v>
+      </c>
+      <c r="C190" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D190" s="4">
+        <v>10</v>
+      </c>
+      <c r="E190" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F190" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G190" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A191" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B191" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C191" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D191" s="4">
+        <v>10</v>
+      </c>
+      <c r="E191" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F191" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G191" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A192" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B192" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C192" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D192" s="4">
+        <v>10</v>
+      </c>
+      <c r="E192" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F192" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G192" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A193" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B193" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C193" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D193" s="4">
+        <v>10</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G193" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A194" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B194" s="6">
+        <v>326</v>
+      </c>
+      <c r="C194" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D194" s="4">
+        <v>10</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F194" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G194" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A195" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B195" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C195" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D195" s="4">
+        <v>10</v>
+      </c>
+      <c r="E195" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F195" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G195" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A196" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B196" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C196" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D196" s="4">
+        <v>10</v>
+      </c>
+      <c r="E196" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F196" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G196" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A197" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B197" s="6">
+        <v>4163214</v>
+      </c>
+      <c r="C197" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D197" s="4">
+        <v>10</v>
+      </c>
+      <c r="E197" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F197" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G197" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A198" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B198" s="6">
+        <v>503853</v>
+      </c>
+      <c r="C198" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D198" s="4">
+        <v>10</v>
+      </c>
+      <c r="E198" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F198" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G198" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A199" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B199" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C199" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D199" s="4">
+        <v>10</v>
+      </c>
+      <c r="E199" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F199" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G199" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A200" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C200" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D200" s="4">
+        <v>10</v>
+      </c>
+      <c r="E200" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F200" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G200" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A201" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B201" s="6">
+        <v>503852</v>
+      </c>
+      <c r="C201" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D201" s="4">
+        <v>10</v>
+      </c>
+      <c r="E201" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F201" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G201" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A202" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B202" s="6">
+        <v>550197</v>
+      </c>
+      <c r="C202" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D202" s="4">
+        <v>10</v>
+      </c>
+      <c r="E202" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F202" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G202" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+      <c r="A203" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B203" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C203" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D203" s="4">
+        <v>10</v>
+      </c>
+      <c r="E203" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F203" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G203" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A204" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C204" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D204" s="4">
+        <v>10</v>
+      </c>
+      <c r="E204" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F204" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G204" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A205" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B205" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C205" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D205" s="4">
+        <v>10</v>
+      </c>
+      <c r="E205" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G205" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A206" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D206" s="4">
+        <v>10</v>
+      </c>
+      <c r="E206" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F206" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G206" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A207" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B207" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D207" s="4">
+        <v>10</v>
+      </c>
+      <c r="E207" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F207" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G207" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A208" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B208" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D208" s="4">
+        <v>10</v>
+      </c>
+      <c r="E208" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F208" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G208" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A209" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D209" s="4">
+        <v>10</v>
+      </c>
+      <c r="E209" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F209" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G209" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A210" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B210" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D210" s="4">
+        <v>10</v>
+      </c>
+      <c r="E210" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F210" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G210" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A211" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B211" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D211" s="4">
+        <v>10</v>
+      </c>
+      <c r="E211" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F211" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G211" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A212" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D212" s="4">
+        <v>10</v>
+      </c>
+      <c r="E212" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G212" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A213" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B213" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D213" s="4">
+        <v>10</v>
+      </c>
+      <c r="E213" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F213" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G213" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A214" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B214" s="6">
+        <v>5030850</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D214" s="4">
+        <v>10</v>
+      </c>
+      <c r="E214" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F214" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G214" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A215" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B215" s="6">
+        <v>5030850</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D215" s="4">
+        <v>10</v>
+      </c>
+      <c r="E215" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F215" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G215" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A216" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D216" s="4">
+        <v>10</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F216" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G216" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A217" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D217" s="4">
+        <v>10</v>
+      </c>
+      <c r="E217" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F217" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G217" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A218" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D218" s="4">
+        <v>10</v>
+      </c>
+      <c r="E218" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F218" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G218" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A219" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B219" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D219" s="4">
+        <v>10</v>
+      </c>
+      <c r="E219" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F219" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G219" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A220" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D220" s="4">
+        <v>10</v>
+      </c>
+      <c r="E220" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F220" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G220" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A221" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C221" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D221" s="4">
+        <v>10</v>
+      </c>
+      <c r="E221" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F221" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G221" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A222" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B222" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C222" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D222" s="4">
+        <v>10</v>
+      </c>
+      <c r="E222" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F222" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G222" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A223" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C223" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D223" s="4">
+        <v>10</v>
+      </c>
+      <c r="E223" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F223" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G223" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A224" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C224" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D224" s="4">
+        <v>10</v>
+      </c>
+      <c r="E224" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F224" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G224" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A225" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B225" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C225" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D225" s="4">
+        <v>10</v>
+      </c>
+      <c r="E225" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F225" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G225" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A226" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B226" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C226" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D226" s="4">
+        <v>10</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F226" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G226" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A227" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C227" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D227" s="4">
+        <v>10</v>
+      </c>
+      <c r="E227" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F227" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G227" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A228" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C228" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D228" s="4">
+        <v>10</v>
+      </c>
+      <c r="E228" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F228" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G228" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A229" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C229" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D229" s="4">
+        <v>10</v>
+      </c>
+      <c r="E229" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F229" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G229" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A230" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C230" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D230" s="4">
+        <v>10</v>
+      </c>
+      <c r="E230" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F230" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G230" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A231" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B231" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C231" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D231" s="4">
+        <v>10</v>
+      </c>
+      <c r="E231" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F231" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G231" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A232" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B232" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C232" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D232" s="4">
+        <v>10</v>
+      </c>
+      <c r="E232" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F232" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G232" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A233" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B233" s="6">
+        <v>6005500030</v>
+      </c>
+      <c r="C233" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D233" s="4">
+        <v>10</v>
+      </c>
+      <c r="E233" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F233" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G233" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A234" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B234" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C234" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D234" s="4">
+        <v>10</v>
+      </c>
+      <c r="E234" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F234" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G234" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A235" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B235" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C235" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D235" s="4">
+        <v>10</v>
+      </c>
+      <c r="E235" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F235" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G235" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A236" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C236" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D236" s="4">
+        <v>10</v>
+      </c>
+      <c r="E236" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F236" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G236" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A237" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B237" s="6">
+        <v>326</v>
+      </c>
+      <c r="C237" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D237" s="4">
+        <v>10</v>
+      </c>
+      <c r="E237" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F237" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G237" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A238" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B238" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C238" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D238" s="4">
+        <v>10</v>
+      </c>
+      <c r="E238" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F238" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G238" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A239" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B239" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C239" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D239" s="4">
+        <v>10</v>
+      </c>
+      <c r="E239" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F239" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G239" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A240" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B240" s="6">
+        <v>4163214</v>
+      </c>
+      <c r="C240" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D240" s="4">
+        <v>10</v>
+      </c>
+      <c r="E240" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F240" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G240" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A241" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B241" s="6">
+        <v>503853</v>
+      </c>
+      <c r="C241" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D241" s="4">
+        <v>10</v>
+      </c>
+      <c r="E241" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F241" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G241" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A242" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C242" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D242" s="4">
+        <v>10</v>
+      </c>
+      <c r="E242" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F242" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G242" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A243" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B243" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C243" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D243" s="4">
+        <v>10</v>
+      </c>
+      <c r="E243" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G243" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A244" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B244" s="6">
+        <v>503852</v>
+      </c>
+      <c r="C244" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="D244" s="4">
+        <v>10</v>
+      </c>
+      <c r="E244" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G244" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A245" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B245" s="6">
+        <v>550197</v>
+      </c>
+      <c r="C245" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D245" s="4">
+        <v>10</v>
+      </c>
+      <c r="E245" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G245" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+      <c r="A246" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B246" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C246" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D246" s="4">
+        <v>10</v>
+      </c>
+      <c r="E246" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G246" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A247" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B247" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C247" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D247" s="4">
+        <v>10</v>
+      </c>
+      <c r="E247" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G247" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A248" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C248" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D248" s="4">
+        <v>10</v>
+      </c>
+      <c r="E248" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F248" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G248" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A249" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C249" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D249" s="4">
+        <v>10</v>
+      </c>
+      <c r="E249" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G249" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A250" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C250" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D250" s="4">
+        <v>10</v>
+      </c>
+      <c r="E250" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="F250" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G250" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A251" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C251" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D251" s="4">
+        <v>10</v>
+      </c>
+      <c r="E251" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F251" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G251" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A252" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C252" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D252" s="4">
+        <v>10</v>
+      </c>
+      <c r="E252" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G252" s="17">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3718,8 +6869,104 @@
     <hyperlink ref="A113" r:id="rId66" tooltip="Bộ dây truyền chống gập màu vàng kèm túi chứa dịch giảm đau 100ml dùng cho máy Rythmic Evolution" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67aa&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
     <hyperlink ref="A114" r:id="rId67" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
     <hyperlink ref="A115" r:id="rId68" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A133" r:id="rId69" tooltip="Vít mắt cá chân đường kính 4.5mm" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ee&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A135" r:id="rId70" tooltip="Vi ống thông Asahi Tellus" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ea&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A136" r:id="rId71" tooltip="Vít xốp đường kính 6.5, ren 32 mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e8&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A138" r:id="rId72" tooltip="Vi ống thông can thiệp Asahi Masters PARKWAY HF KIT" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e4&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A140" r:id="rId73" tooltip="Vít xương cứng đường kính 4.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e0&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A141" r:id="rId74" tooltip="Vít xương cứng đường kính 3.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68de&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A142" r:id="rId75" tooltip="Khẩu trang 3 lớp hộp 55 cái" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68dc"/>
+    <hyperlink ref="A144" r:id="rId76" tooltip="Nẹp DCP, vít 3.5mm, 8~12 lỗ" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A146" r:id="rId77" tooltip="Dây cho ăn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d4&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A147" r:id="rId78" tooltip="Túi ép tiệt trùng Tyvek" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68cc&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A148" r:id="rId79" tooltip="Thông hậu môn (Rectal)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A149" r:id="rId80" tooltip="Dây thông T" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c6&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A151" r:id="rId81" tooltip="Nẹp khóa đa hướng đầu trên mâm chày (trái, phải)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c2&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A152" r:id="rId82" tooltip="Bộ túi máu rỗng 150 mL (4 túi)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cf&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A153" r:id="rId83" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cd&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A154" r:id="rId84" tooltip="CERTOFIX TRIO V 720" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cb&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A155" r:id="rId85" tooltip="Urgostart Micro-Adhesive 10cm x 10cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c9&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A156" r:id="rId86" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c7&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A157" r:id="rId87" tooltip="Thông foley 3 nhánh" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c5&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A158" r:id="rId88" tooltip="Urgostart Micro-Adhesive 6cm x 6cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c3&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A159" r:id="rId89" tooltip="Urgostart Contact 5cm x 7cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c1&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A160" r:id="rId90" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Chỉ kèm miếng đệm Pledget 7x3x1,5mm." display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bf&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A161" r:id="rId91" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Đóng gói Multipack" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bd&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A162" r:id="rId92" tooltip="Chỉ không tan tổng hợp đơn sợi Surgipro số 7-0 dài 60, 2 kim tròn đầu cắt KV-11, 3/8C, 9mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bb&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A163" r:id="rId93" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b9&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A164" r:id="rId94" tooltip="Nẹp khóa xương đòn, móc xương đòn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b6&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A165" r:id="rId95" tooltip="Túi máu đơn Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b4&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A166" r:id="rId96" tooltip="Túi máu đôi Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67b2&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A167" r:id="rId97" tooltip="Thông foley 2 nhánh" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67b0&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A168" r:id="rId98" tooltip="Nẹp khóa ốp lồi cầu đùi" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67ae&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A169" r:id="rId99" tooltip="Bộ dây truyền chống gập màu vàng kèm túi chứa dịch giảm đau 200ml dùng cho máy Rythmic Evolution" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67ac&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A170" r:id="rId100" tooltip="Bộ dây truyền chống gập màu vàng kèm túi chứa dịch giảm đau 100ml dùng cho máy Rythmic Evolution" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67aa&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A171" r:id="rId101" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A172" r:id="rId102" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A176" r:id="rId103" tooltip="Vít mắt cá chân đường kính 4.5mm" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ee&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A178" r:id="rId104" tooltip="Vi ống thông Asahi Tellus" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ea&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A179" r:id="rId105" tooltip="Vít xốp đường kính 6.5, ren 32 mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e8&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A181" r:id="rId106" tooltip="Vi ống thông can thiệp Asahi Masters PARKWAY HF KIT" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e4&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A183" r:id="rId107" tooltip="Vít xương cứng đường kính 4.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e0&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A184" r:id="rId108" tooltip="Vít xương cứng đường kính 3.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68de&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A185" r:id="rId109" tooltip="Khẩu trang 3 lớp hộp 55 cái" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68dc"/>
+    <hyperlink ref="A187" r:id="rId110" tooltip="Nẹp DCP, vít 3.5mm, 8~12 lỗ" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A189" r:id="rId111" tooltip="Dây cho ăn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d4&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A190" r:id="rId112" tooltip="Túi ép tiệt trùng Tyvek" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68cc&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A191" r:id="rId113" tooltip="Thông hậu môn (Rectal)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A192" r:id="rId114" tooltip="Dây thông T" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c6&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A194" r:id="rId115" tooltip="Nẹp khóa đa hướng đầu trên mâm chày (trái, phải)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c2&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A195" r:id="rId116" tooltip="Bộ túi máu rỗng 150 mL (4 túi)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cf&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A196" r:id="rId117" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cd&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A197" r:id="rId118" tooltip="CERTOFIX TRIO V 720" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cb&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A198" r:id="rId119" tooltip="Urgostart Micro-Adhesive 10cm x 10cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c9&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A199" r:id="rId120" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c7&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A200" r:id="rId121" tooltip="Thông foley 3 nhánh" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c5&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A201" r:id="rId122" tooltip="Urgostart Micro-Adhesive 6cm x 6cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c3&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A202" r:id="rId123" tooltip="Urgostart Contact 5cm x 7cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c1&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A203" r:id="rId124" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Chỉ kèm miếng đệm Pledget 7x3x1,5mm." display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bf&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A204" r:id="rId125" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Đóng gói Multipack" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bd&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A205" r:id="rId126" tooltip="Chỉ không tan tổng hợp đơn sợi Surgipro số 7-0 dài 60, 2 kim tròn đầu cắt KV-11, 3/8C, 9mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bb&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A206" r:id="rId127" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b9&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A207" r:id="rId128" tooltip="Nẹp khóa xương đòn, móc xương đòn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b6&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A208" r:id="rId129" tooltip="Túi máu đơn Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b4&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A209" r:id="rId130" tooltip="Túi máu đôi Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67b2&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A210" r:id="rId131" tooltip="Thông foley 2 nhánh" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67b0&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A211" r:id="rId132" tooltip="Nẹp khóa ốp lồi cầu đùi" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67ae&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A212" r:id="rId133" tooltip="Bộ dây truyền chống gập màu vàng kèm túi chứa dịch giảm đau 200ml dùng cho máy Rythmic Evolution" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67ac&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A213" r:id="rId134" tooltip="Bộ dây truyền chống gập màu vàng kèm túi chứa dịch giảm đau 100ml dùng cho máy Rythmic Evolution" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67aa&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A214" r:id="rId135" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A215" r:id="rId136" tooltip="Chăn làm ấm phẫu thuật trẻ em WarmTouch cỡ 63x104cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67a8&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A219" r:id="rId137" tooltip="Vít mắt cá chân đường kính 4.5mm" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ee&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A221" r:id="rId138" tooltip="Vi ống thông Asahi Tellus" display="http://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68ea&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A222" r:id="rId139" tooltip="Vít xốp đường kính 6.5, ren 32 mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e8&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A224" r:id="rId140" tooltip="Vi ống thông can thiệp Asahi Masters PARKWAY HF KIT" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e4&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A226" r:id="rId141" tooltip="Vít xương cứng đường kính 4.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68e0&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A227" r:id="rId142" tooltip="Vít xương cứng đường kính 3.5mm, tự taro" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68de&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A228" r:id="rId143" tooltip="Khẩu trang 3 lớp hộp 55 cái" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68dc"/>
+    <hyperlink ref="A230" r:id="rId144" tooltip="Nẹp DCP, vít 3.5mm, 8~12 lỗ" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A232" r:id="rId145" tooltip="Dây cho ăn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68d4&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A233" r:id="rId146" tooltip="Túi ép tiệt trùng Tyvek" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68cc&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A234" r:id="rId147" tooltip="Thông hậu môn (Rectal)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c8&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A235" r:id="rId148" tooltip="Dây thông T" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c6&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A237" r:id="rId149" tooltip="Nẹp khóa đa hướng đầu trên mâm chày (trái, phải)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78afffdf9a12984a68c2&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A238" r:id="rId150" tooltip="Bộ túi máu rỗng 150 mL (4 túi)" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cf&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A239" r:id="rId151" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cd&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A240" r:id="rId152" tooltip="CERTOFIX TRIO V 720" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67cb&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A241" r:id="rId153" tooltip="Urgostart Micro-Adhesive 10cm x 10cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c9&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A242" r:id="rId154" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c7&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A243" r:id="rId155" tooltip="Thông foley 3 nhánh" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c5&amp;categoryId=5f9bc61ca5bf323cf13ecc15"/>
+    <hyperlink ref="A244" r:id="rId156" tooltip="Urgostart Micro-Adhesive 6cm x 6cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c3&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A245" r:id="rId157" tooltip="Urgostart Contact 5cm x 7cm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67c1&amp;categoryId=5f9bc4e35c52b2593d16de25"/>
+    <hyperlink ref="A246" r:id="rId158" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Chỉ kèm miếng đệm Pledget 7x3x1,5mm." display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bf&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A247" r:id="rId159" tooltip="Chỉ không tan tổng hợp sợi bên Ticron số 2-0 dài 75, 2 kim tròn đầu nhọn CV-316, 1/2C, 20mm. Đóng gói Multipack" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bd&amp;categoryId=5f9bc50c4c653c5c706c3d85"/>
+    <hyperlink ref="A248" r:id="rId160" tooltip="Chỉ không tan tổng hợp đơn sợi Surgipro số 7-0 dài 60, 2 kim tròn đầu cắt KV-11, 3/8C, 9mm" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67bb&amp;categoryId=5f9bc57da7307960eb32bb63"/>
+    <hyperlink ref="A249" r:id="rId161" tooltip="Chất nhầy nhãn khoa" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b9&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A250" r:id="rId162" tooltip="Nẹp khóa xương đòn, móc xương đòn" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b6&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A251" r:id="rId163" tooltip="Túi máu đơn Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78acffdf9a12984a67b4&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
+    <hyperlink ref="A252" r:id="rId164" tooltip="Túi máu đôi Demotek 250mL" display="https://congkhaiyte.moh.gov.vn/?page=Project.MedicalPrice.Home.MedicalPrice.Material.detail&amp;id=611f78abffdf9a12984a67b2&amp;categoryId=5f9bc540c5dbc2404e1d7e23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId69"/>
+  <pageSetup orientation="portrait" r:id="rId165"/>
 </worksheet>
 </file>
</xml_diff>